<commit_message>
Updated int repeats and analyzed btwn barrel figures for v5swap
</commit_message>
<xml_diff>
--- a/OverlapingHomologues.xlsx
+++ b/OverlapingHomologues.xlsx
@@ -1,27 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10523"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meghan/Documents/PhD/v6_2018/OMBBNetwork/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meghan/Documents/PhD/GitHubProjects/v6_2018_Network/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4B1BDFEA-03ED-CC44-8B3B-84277A970B7D}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{091C6C4B-8114-D64A-AA7C-B7E76597A734}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30180" yWindow="1020" windowWidth="28040" windowHeight="16500" xr2:uid="{153AAEF5-0600-D14C-98A0-EDC583A10DD1}"/>
+    <workbookView xWindow="13460" yWindow="4720" windowWidth="31940" windowHeight="17940" xr2:uid="{153AAEF5-0600-D14C-98A0-EDC583A10DD1}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="v5" sheetId="1" r:id="rId1"/>
+    <sheet name="v5Swap" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -374,7 +379,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -587,4 +592,602 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04E448A0-613C-2245-AF23-7AFC4BF77EB4}">
+  <dimension ref="A1:P17"/>
+  <sheetViews>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData>
+    <row r="1" spans="1:16">
+      <c r="B1">
+        <v>8</v>
+      </c>
+      <c r="C1">
+        <v>10</v>
+      </c>
+      <c r="D1">
+        <v>12</v>
+      </c>
+      <c r="E1">
+        <v>14</v>
+      </c>
+      <c r="F1">
+        <v>16</v>
+      </c>
+      <c r="G1">
+        <v>18</v>
+      </c>
+      <c r="H1">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16">
+      <c r="A2">
+        <v>8</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>11</v>
+      </c>
+      <c r="D2">
+        <v>306</v>
+      </c>
+      <c r="E2">
+        <v>41</v>
+      </c>
+      <c r="F2">
+        <v>82</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
+      <c r="A3">
+        <v>10</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
+      <c r="A4">
+        <v>12</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <v>23</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
+      <c r="A5">
+        <v>14</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>44</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16">
+      <c r="A6">
+        <v>16</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>83</v>
+      </c>
+      <c r="H6">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16">
+      <c r="A7">
+        <v>18</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16">
+      <c r="A8">
+        <v>22</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16">
+      <c r="A11">
+        <v>8</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>1.32084534102E-3</v>
+      </c>
+      <c r="D11">
+        <v>3.6743515850100002E-2</v>
+      </c>
+      <c r="E11">
+        <v>4.9231508165200003E-3</v>
+      </c>
+      <c r="F11">
+        <v>9.8463016330499996E-3</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>2.4015369836700002E-3</v>
+      </c>
+      <c r="J11">
+        <f>B11*100</f>
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <f t="shared" ref="K11:P11" si="0">C11*100</f>
+        <v>0.132084534102</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="0"/>
+        <v>3.6743515850100001</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="0"/>
+        <v>0.49231508165200005</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="0"/>
+        <v>0.98463016330499997</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <f t="shared" si="0"/>
+        <v>0.24015369836700001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>4.6012269938700001E-3</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <f t="shared" ref="J12:J18" si="1">B12*100</f>
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <f t="shared" ref="K12:K18" si="2">C12*100</f>
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <f t="shared" ref="L12:L18" si="3">D12*100</f>
+        <v>0.46012269938700001</v>
+      </c>
+      <c r="M12">
+        <f t="shared" ref="M12:M18" si="4">E12*100</f>
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <f t="shared" ref="N12:N18" si="5">F12*100</f>
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <f t="shared" ref="O12:O18" si="6">G12*100</f>
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <f t="shared" ref="P12:P18" si="7">H12*100</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>2.0691082143600001E-4</v>
+      </c>
+      <c r="F13">
+        <v>2.3794744465099999E-3</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>4.1382164287200003E-4</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="4"/>
+        <v>2.0691082143600003E-2</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="5"/>
+        <v>0.23794744465099998</v>
+      </c>
+      <c r="O13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="P13">
+        <f t="shared" si="7"/>
+        <v>4.1382164287200006E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16">
+      <c r="A14">
+        <v>14</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>1.5083990401100001E-2</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>1.4055536510100001E-2</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="5"/>
+        <v>1.50839904011</v>
+      </c>
+      <c r="O14">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="P14">
+        <f t="shared" si="7"/>
+        <v>1.4055536510100002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16">
+      <c r="A15">
+        <v>16</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>1.39285114952E-2</v>
+      </c>
+      <c r="H15">
+        <v>2.1815740896099999E-3</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <f t="shared" si="6"/>
+        <v>1.39285114952</v>
+      </c>
+      <c r="P15">
+        <f t="shared" si="7"/>
+        <v>0.218157408961</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16">
+      <c r="A16">
+        <v>18</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N16">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="P16">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16">
+      <c r="A17">
+        <v>22</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N17">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="P17">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>